<commit_message>
articulation patterns part 2. 1 more endpoint, w is recognized
</commit_message>
<xml_diff>
--- a/src/main/java/phonosemantics/input/PhonemesCoverageExample.xlsx
+++ b/src/main/java/phonosemantics/input/PhonemesCoverageExample.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07977ED6-FFCC-4D29-B2AC-983FB8C8C15F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="3912" yWindow="1356" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vowels" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="212">
   <si>
     <t>Close</t>
   </si>
@@ -648,12 +649,15 @@
   </si>
   <si>
     <t>ɭ̊˔</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -663,7 +667,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +677,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -785,22 +795,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -816,9 +827,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -856,7 +867,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -891,6 +902,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -926,9 +954,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1101,38 +1146,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1152,7 +1197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1192,7 +1237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1215,7 +1260,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1231,7 +1276,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1254,7 +1299,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +1314,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1290,18 +1335,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F16" s="9"/>
     </row>
   </sheetData>
@@ -1315,108 +1360,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="25" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="25" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11" t="s">
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-    </row>
-    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+    </row>
+    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14" t="s">
+      <c r="K2" s="17"/>
+      <c r="L2" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14" t="s">
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14" t="s">
+      <c r="O2" s="17"/>
+      <c r="P2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14" t="s">
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14" t="s">
+      <c r="S2" s="17"/>
+      <c r="T2" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14" t="s">
+      <c r="W2" s="17"/>
+      <c r="X2" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="12"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="11"/>
       <c r="AA2" s="9"/>
       <c r="AB2" s="9"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
@@ -1458,13 +1503,13 @@
       <c r="U3" t="s">
         <v>153</v>
       </c>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
@@ -1506,22 +1551,22 @@
       <c r="V4" t="s">
         <v>159</v>
       </c>
-      <c r="W4" s="15"/>
+      <c r="W4" s="13"/>
       <c r="X4" t="s">
         <v>160</v>
       </c>
-      <c r="Y4" s="15"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="Y4" s="13"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
       <c r="J5" t="s">
         <v>94</v>
       </c>
@@ -1540,17 +1585,17 @@
       <c r="O5" t="s">
         <v>99</v>
       </c>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
@@ -1605,16 +1650,16 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
       <c r="J7" t="s">
         <v>74</v>
       </c>
@@ -1639,17 +1684,17 @@
       <c r="Q7" t="s">
         <v>172</v>
       </c>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
         <v>93</v>
       </c>
       <c r="B8" t="s">
@@ -1664,28 +1709,28 @@
       <c r="E8" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="15" t="s">
         <v>126</v>
       </c>
       <c r="O8" t="s">
@@ -1697,34 +1742,37 @@
       <c r="Q8" t="s">
         <v>174</v>
       </c>
-      <c r="R8" s="16" t="s">
+      <c r="R8" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="S8" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="T8" s="16" t="s">
+      <c r="T8" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="U8" s="16" t="s">
+      <c r="U8" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="V8" s="16" t="s">
+      <c r="V8" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="W8" s="16" t="s">
+      <c r="W8" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="X8" s="16" t="s">
+      <c r="X8" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="Y8" s="16" t="s">
+      <c r="Y8" s="14" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
         <v>49</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>211</v>
       </c>
       <c r="D9" t="s">
         <v>128</v>
@@ -1732,10 +1780,10 @@
       <c r="E9" t="s">
         <v>129</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="15" t="s">
         <v>131</v>
       </c>
       <c r="N9" t="s">
@@ -1750,18 +1798,18 @@
       <c r="Q9" t="s">
         <v>183</v>
       </c>
-      <c r="R9" s="16" t="s">
+      <c r="R9" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="S9" s="14" t="s">
         <v>181</v>
       </c>
       <c r="Y9" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C10" t="s">
@@ -1773,10 +1821,10 @@
       <c r="G10" t="s">
         <v>135</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="15" t="s">
         <v>137</v>
       </c>
       <c r="N10" t="s">
@@ -1785,19 +1833,19 @@
       <c r="O10" t="s">
         <v>139</v>
       </c>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
       <c r="U10" t="s">
         <v>185</v>
       </c>
       <c r="W10" t="s">
         <v>186</v>
       </c>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B11" t="s">
@@ -1806,10 +1854,10 @@
       <c r="C11" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="15" t="s">
         <v>79</v>
       </c>
       <c r="N11" t="s">
@@ -1818,8 +1866,8 @@
       <c r="O11" t="s">
         <v>142</v>
       </c>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
       <c r="T11" t="s">
         <v>190</v>
       </c>
@@ -1832,21 +1880,21 @@
       <c r="W11" t="s">
         <v>187</v>
       </c>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="J12" s="17" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="J12" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="15" t="s">
         <v>144</v>
       </c>
       <c r="N12" t="s">
@@ -1861,23 +1909,23 @@
       <c r="S12" t="s">
         <v>191</v>
       </c>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="J13" s="17" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="J13" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="15" t="s">
         <v>146</v>
       </c>
       <c r="N13" t="s">
@@ -1898,23 +1946,23 @@
       <c r="S13" t="s">
         <v>193</v>
       </c>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="J14" s="17" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="J14" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="15" t="s">
         <v>76</v>
       </c>
       <c r="N14" t="s">
@@ -1938,20 +1986,20 @@
       <c r="U14" t="s">
         <v>198</v>
       </c>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="K15" s="17" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="K15" s="15" t="s">
         <v>148</v>
       </c>
       <c r="O15" t="s">
@@ -1963,13 +2011,18 @@
       <c r="S15" t="s">
         <v>197</v>
       </c>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="V1:Y1"/>
@@ -1980,11 +2033,6 @@
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="G1:P1"/>
     <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
in progress classes 2022 added, old deprecated
</commit_message>
<xml_diff>
--- a/src/main/java/phonosemantics/input/PhonemesCoverageExample.xlsx
+++ b/src/main/java/phonosemantics/input/PhonemesCoverageExample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="1350" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="3915" yWindow="1350" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Vowels" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="216">
   <si>
     <t>Close</t>
   </si>
@@ -651,6 +651,18 @@
   </si>
   <si>
     <t>tʃ</t>
+  </si>
+  <si>
+    <t>ĩ</t>
+  </si>
+  <si>
+    <t>ẽ</t>
+  </si>
+  <si>
+    <t>ã</t>
+  </si>
+  <si>
+    <t>õ</t>
   </si>
 </sst>
 </file>
@@ -719,17 +731,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -784,11 +785,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -797,19 +811,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -838,11 +849,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1146,215 +1169,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:9">
+      <c r="B1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="19"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="3" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="I5" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="1"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="I9" s="7"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="E13" s="9"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="F16" s="9"/>
+    <row r="12" spans="1:9">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="F13" s="8"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="G16" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1362,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
@@ -1373,94 +1425,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
     </row>
     <row r="2" spans="1:28" ht="30" customHeight="1">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="21" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="22"/>
-      <c r="T2" s="20" t="s">
+      <c r="S2" s="21"/>
+      <c r="T2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20" t="s">
+      <c r="U2" s="19"/>
+      <c r="V2" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20" t="s">
+      <c r="W2" s="19"/>
+      <c r="X2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
@@ -1502,13 +1554,13 @@
       <c r="U3" t="s">
         <v>151</v>
       </c>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
@@ -1538,7 +1590,7 @@
       <c r="R4" t="s">
         <v>153</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="S4" s="16" t="s">
         <v>154</v>
       </c>
       <c r="T4" t="s">
@@ -1550,22 +1602,22 @@
       <c r="V4" t="s">
         <v>157</v>
       </c>
-      <c r="W4" s="13"/>
+      <c r="W4" s="12"/>
       <c r="X4" t="s">
         <v>158</v>
       </c>
-      <c r="Y4" s="13"/>
+      <c r="Y4" s="12"/>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
       <c r="J5" t="s">
         <v>94</v>
       </c>
@@ -1584,17 +1636,17 @@
       <c r="O5" t="s">
         <v>97</v>
       </c>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
@@ -1636,7 +1688,7 @@
       <c r="R6" t="s">
         <v>166</v>
       </c>
-      <c r="S6" s="17" t="s">
+      <c r="S6" s="16" t="s">
         <v>165</v>
       </c>
       <c r="T6" t="s">
@@ -1650,15 +1702,15 @@
       </c>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="J7" t="s">
         <v>74</v>
       </c>
@@ -1683,17 +1735,17 @@
       <c r="Q7" t="s">
         <v>170</v>
       </c>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B8" t="s">
@@ -1708,28 +1760,28 @@
       <c r="E8" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="14" t="s">
         <v>124</v>
       </c>
       <c r="O8" t="s">
@@ -1741,36 +1793,36 @@
       <c r="Q8" t="s">
         <v>172</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="R8" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="S8" s="18" t="s">
+      <c r="S8" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="T8" s="14" t="s">
+      <c r="T8" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="U8" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="V8" s="14" t="s">
+      <c r="V8" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="W8" s="14" t="s">
+      <c r="W8" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="X8" s="14" t="s">
+      <c r="X8" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="14" t="s">
+      <c r="Y8" s="13" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:28">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>209</v>
       </c>
       <c r="D9" t="s">
@@ -1779,10 +1831,10 @@
       <c r="E9" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="14" t="s">
         <v>129</v>
       </c>
       <c r="N9" t="s">
@@ -1797,10 +1849,10 @@
       <c r="Q9" t="s">
         <v>181</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="R9" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="S9" s="18" t="s">
+      <c r="S9" s="17" t="s">
         <v>179</v>
       </c>
       <c r="Y9" t="s">
@@ -1808,7 +1860,7 @@
       </c>
     </row>
     <row r="10" spans="1:28">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C10" t="s">
@@ -1820,10 +1872,10 @@
       <c r="G10" t="s">
         <v>133</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="14" t="s">
         <v>135</v>
       </c>
       <c r="N10" t="s">
@@ -1832,19 +1884,19 @@
       <c r="O10" t="s">
         <v>137</v>
       </c>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
       <c r="U10" t="s">
         <v>183</v>
       </c>
       <c r="W10" t="s">
         <v>184</v>
       </c>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
     </row>
     <row r="11" spans="1:28">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B11" t="s">
@@ -1853,10 +1905,10 @@
       <c r="C11" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>79</v>
       </c>
       <c r="N11" t="s">
@@ -1865,8 +1917,8 @@
       <c r="O11" t="s">
         <v>140</v>
       </c>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
       <c r="T11" t="s">
         <v>188</v>
       </c>
@@ -1879,21 +1931,21 @@
       <c r="W11" t="s">
         <v>185</v>
       </c>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="J12" s="15" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="J12" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="14" t="s">
         <v>142</v>
       </c>
       <c r="N12" t="s">
@@ -1905,26 +1957,26 @@
       <c r="R12" t="s">
         <v>190</v>
       </c>
-      <c r="S12" s="17" t="s">
+      <c r="S12" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="J13" s="15" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="J13" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="14" t="s">
         <v>144</v>
       </c>
       <c r="N13" t="s">
@@ -1942,26 +1994,26 @@
       <c r="R13" t="s">
         <v>192</v>
       </c>
-      <c r="S13" s="17" t="s">
+      <c r="S13" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
     </row>
     <row r="14" spans="1:28">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="J14" s="15" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="J14" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>76</v>
       </c>
       <c r="N14" t="s">
@@ -1979,26 +2031,26 @@
       <c r="R14" t="s">
         <v>194</v>
       </c>
-      <c r="S14" s="17" t="s">
+      <c r="S14" s="16" t="s">
         <v>193</v>
       </c>
       <c r="U14" t="s">
         <v>196</v>
       </c>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="K15" s="15" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="K15" s="14" t="s">
         <v>146</v>
       </c>
       <c r="O15" t="s">
@@ -2007,16 +2059,21 @@
       <c r="Q15" t="s">
         <v>203</v>
       </c>
-      <c r="S15" s="17" t="s">
+      <c r="S15" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="V1:Y1"/>
@@ -2028,11 +2085,6 @@
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="R2:S2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>